<commit_message>
Added time constraint and cross docking constraint
</commit_message>
<xml_diff>
--- a/input_data/orders.xlsx
+++ b/input_data/orders.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinehagen/PycharmProjects/chris/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinesorli/Chris-Tora-master/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8664D90B-E0D1-264A-87F6-7BEF28D5B0DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="1540" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{12B052AB-01B4-4242-9AB3-FAFF58C5AB0B}"/>
+    <workbookView xWindow="5560" yWindow="1540" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Ordrenr</t>
   </si>
@@ -81,12 +86,15 @@
   </si>
   <si>
     <t>price</t>
+  </si>
+  <si>
+    <t>contract</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -441,11 +449,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5E1E78-2B73-FD41-8984-CDD57CE8E2D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,7 +556,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E5" s="3">
         <v>3</v>
@@ -563,11 +571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC730145-1AD2-5B4C-A231-B6C451137B72}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,7 +604,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -616,7 +624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87DE97C-C702-0142-8F76-8E4C7630A9F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Only product type 1-2 and 2-3
</commit_message>
<xml_diff>
--- a/input_data/orders.xlsx
+++ b/input_data/orders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinehagen/PycharmProjects/chris/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8EA8A2-2788-CC4A-B5B4-757C9ECA4892}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D3ECB1-08E4-B74F-A14B-8436D869397B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="800" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="800" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>Ordrenr</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>ChrisKunden</t>
-  </si>
-  <si>
-    <t>fisk3til4</t>
   </si>
   <si>
     <t>Utenfor landet</t>
@@ -447,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,10 +471,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -585,10 +582,10 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -599,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -610,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -620,10 +617,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,10 +634,10 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -670,10 +667,21 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed parameter values to test customer constraint
</commit_message>
<xml_diff>
--- a/input_data/orders.xlsx
+++ b/input_data/orders.xlsx
@@ -1,32 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinehagen/PycharmProjects/chris/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinesorli/Chris-Tora-master/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D3ECB1-08E4-B74F-A14B-8436D869397B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="800" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="800" windowWidth="28040" windowHeight="17440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -86,7 +85,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -441,11 +440,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F2" s="2">
         <v>57</v>
@@ -511,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F3" s="2">
         <v>63</v>
@@ -531,7 +530,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F4">
         <v>34</v>
@@ -545,13 +544,13 @@
         <v>84752</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>864</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <v>63</v>
@@ -563,11 +562,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,7 +595,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -607,7 +606,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -616,10 +615,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Link til vendor excel
</commit_message>
<xml_diff>
--- a/input_data/orders.xlsx
+++ b/input_data/orders.xlsx
@@ -1,32 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinehagen/PycharmProjects/chris/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinesorli/Chris-Tora-master/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42679F16-70B0-8A49-81C9-6BE79247231C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="1940" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="1920" windowWidth="28040" windowHeight="17440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -50,12 +49,6 @@
     <t>KristineKunden</t>
   </si>
   <si>
-    <t>fisk1til2</t>
-  </si>
-  <si>
-    <t>fisk2til3</t>
-  </si>
-  <si>
     <t>ChrisKunden</t>
   </si>
   <si>
@@ -81,12 +74,18 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>2-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -125,9 +124,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,18 +440,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.1640625" customWidth="1"/>
     <col min="7" max="7" width="16.1640625" customWidth="1"/>
   </cols>
@@ -471,10 +470,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -487,13 +486,13 @@
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>100</v>
       </c>
     </row>
@@ -507,13 +506,13 @@
       <c r="C3">
         <v>300</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>100</v>
       </c>
     </row>
@@ -527,10 +526,10 @@
       <c r="C4">
         <v>400</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4">
@@ -539,7 +538,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>84752</v>
@@ -547,15 +546,18 @@
       <c r="C5">
         <v>864</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2">
         <v>1</v>
       </c>
       <c r="F5">
         <v>100</v>
       </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -563,7 +565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -582,10 +584,10 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -596,18 +598,18 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -616,11 +618,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,18 +636,18 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -655,8 +657,8 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -664,10 +666,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -675,10 +677,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C5">
         <v>3</v>

</xml_diff>